<commit_message>
Popup handling at profile management
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
+++ b/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE1B336-5155-4A61-9163-F6CF24292725}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <xr:revisionPtr documentId="13_ncr:1_{BDE1B336-5155-4A61-9163-F6CF24292725}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="59">
   <si>
     <t>Date</t>
   </si>
@@ -170,12 +170,37 @@
   </si>
   <si>
     <t>51522379+8</t>
+  </si>
+  <si>
+    <t>51524027</t>
+  </si>
+  <si>
+    <t>51524027+2</t>
+  </si>
+  <si>
+    <t>51524027+3</t>
+  </si>
+  <si>
+    <t>51524027+4</t>
+  </si>
+  <si>
+    <t>51524027+5</t>
+  </si>
+  <si>
+    <t>51524027+6</t>
+  </si>
+  <si>
+    <t>51524027+7</t>
+  </si>
+  <si>
+    <t>51524027+8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="241">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +293,1128 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="240">
     <border>
       <left/>
       <right/>
@@ -446,51 +1591,947 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="140">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="2" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="4" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="6" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="7" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="8" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="9" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="10" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="11" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="12" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="13" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="19" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="21" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="23" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="25" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="27" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="29" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="31" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="33" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="35" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="37" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="47" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="49" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="51" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="53" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="55" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="57" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="59" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="61" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="63" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="65" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="67" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="69" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="71" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="73" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="75" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="77" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="79" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="81" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="83" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="85" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="87" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="89" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="91" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="93" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="95" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="97" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="99" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="101" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="103" fillId="104" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="105" fillId="106" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="107" fillId="108" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="109" fillId="110" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="111" fillId="112" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="113" fillId="114" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="115" fillId="116" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="117" fillId="118" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="119" fillId="120" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="121" fillId="122" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="123" fillId="124" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="125" fillId="126" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="127" fillId="128" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="129" fillId="130" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="131" fillId="132" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="133" fillId="134" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="135" fillId="136" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="137" fillId="138" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="139" fillId="140" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="141" fillId="142" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="143" fillId="144" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="145" fillId="146" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="147" fillId="148" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="149" fillId="150" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="151" fillId="152" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="153" fillId="154" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="155" fillId="156" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="157" fillId="158" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="159" fillId="160" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="161" fillId="162" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="163" fillId="164" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="165" fillId="166" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="167" fillId="168" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="169" fillId="170" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="171" fillId="172" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="173" fillId="174" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="175" fillId="176" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="177" fillId="178" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="179" fillId="180" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="181" fillId="182" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="183" fillId="184" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="185" fillId="186" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="187" fillId="188" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="189" fillId="190" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="191" fillId="192" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="193" fillId="194" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="195" fillId="196" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="197" fillId="198" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="199" fillId="200" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="201" fillId="202" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="203" fillId="204" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="205" fillId="206" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="207" fillId="208" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="209" fillId="210" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="211" fillId="212" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="213" fillId="214" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="215" fillId="216" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="217" fillId="218" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="219" fillId="220" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="221" fillId="222" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="223" fillId="224" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="225" fillId="226" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="227" fillId="228" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="229" fillId="230" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="231" fillId="232" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="233" fillId="234" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="235" fillId="236" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="237" fillId="238" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="240" borderId="239" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -507,10 +2548,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -545,7 +2586,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,7 +2638,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,7 +2743,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -711,13 +2752,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -727,7 +2768,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -736,7 +2777,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -745,7 +2786,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -755,12 +2796,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -791,7 +2832,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -810,7 +2851,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -822,8 +2863,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -831,20 +2872,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" style="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.73046875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.98046875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="6.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="7.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="21.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -901,11 +2942,11 @@
       <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>43</v>
+      <c r="C2" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="126" t="s">
+        <v>51</v>
       </c>
       <c r="E2" s="11">
         <v>1</v>
@@ -948,11 +2989,11 @@
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>43</v>
+      <c r="C3" s="129" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="128" t="s">
+        <v>51</v>
       </c>
       <c r="E3" s="12">
         <v>400</v>
@@ -995,11 +3036,11 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>43</v>
+      <c r="C4" s="131" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="130" t="s">
+        <v>51</v>
       </c>
       <c r="E4" s="12">
         <v>400</v>
@@ -1042,11 +3083,11 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>43</v>
+      <c r="C5" s="133" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="132" t="s">
+        <v>51</v>
       </c>
       <c r="E5" s="12">
         <v>400</v>
@@ -1089,11 +3130,11 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>43</v>
+      <c r="C6" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="134" t="s">
+        <v>51</v>
       </c>
       <c r="E6" s="12">
         <v>156.47999999999999</v>
@@ -1136,11 +3177,11 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>43</v>
+      <c r="C7" s="137" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="136" t="s">
+        <v>51</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
@@ -1183,11 +3224,11 @@
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>43</v>
+      <c r="C8" s="139" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="138" t="s">
+        <v>51</v>
       </c>
       <c r="E8" s="7">
         <v>2000</v>
@@ -1224,13 +3265,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -1238,19 +3279,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="48.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="48.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -1333,12 +3374,12 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1347,6 +3388,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updation of log4j xml
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
+++ b/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -194,6 +194,54 @@
   </si>
   <si>
     <t>51524027+8</t>
+  </si>
+  <si>
+    <t>51524494</t>
+  </si>
+  <si>
+    <t>51524494+2</t>
+  </si>
+  <si>
+    <t>51524494+3</t>
+  </si>
+  <si>
+    <t>51524494+4</t>
+  </si>
+  <si>
+    <t>51524494+5</t>
+  </si>
+  <si>
+    <t>51524494+6</t>
+  </si>
+  <si>
+    <t>51524494+7</t>
+  </si>
+  <si>
+    <t>51524494+8</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+2</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+3</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+4</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+5</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+6</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+7</t>
+  </si>
+  <si>
+    <t>row 2 or column OrderId does not exist in xls+8</t>
   </si>
 </sst>
 </file>
@@ -210,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="241">
+  <fills count="577">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1413,8 +1461,1688 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="240">
+  <borders count="576">
     <border>
       <left/>
       <right/>
@@ -2375,11 +4103,1187 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="308">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
@@ -2525,7 +5429,175 @@
     <xf applyBorder="true" applyFill="true" borderId="233" fillId="234" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="235" fillId="236" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="237" fillId="238" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="240" borderId="239" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="239" fillId="240" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="241" fillId="242" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="243" fillId="244" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="245" fillId="246" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="247" fillId="248" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="249" fillId="250" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="251" fillId="252" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="253" fillId="254" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="255" fillId="256" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="257" fillId="258" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="259" fillId="260" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="261" fillId="262" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="263" fillId="264" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="265" fillId="266" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="267" fillId="268" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="269" fillId="270" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="271" fillId="272" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="273" fillId="274" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="275" fillId="276" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="277" fillId="278" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="279" fillId="280" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="281" fillId="282" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="283" fillId="284" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="285" fillId="286" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="287" fillId="288" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="289" fillId="290" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="291" fillId="292" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="293" fillId="294" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="295" fillId="296" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="297" fillId="298" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="299" fillId="300" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="301" fillId="302" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="303" fillId="304" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="305" fillId="306" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="307" fillId="308" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="309" fillId="310" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="311" fillId="312" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="313" fillId="314" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="315" fillId="316" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="317" fillId="318" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="319" fillId="320" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="321" fillId="322" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="323" fillId="324" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="325" fillId="326" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="327" fillId="328" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="329" fillId="330" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="331" fillId="332" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="333" fillId="334" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="335" fillId="336" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="337" fillId="338" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="339" fillId="340" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="341" fillId="342" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="343" fillId="344" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="345" fillId="346" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="347" fillId="348" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="349" fillId="350" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="351" fillId="352" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="353" fillId="354" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="355" fillId="356" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="357" fillId="358" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="359" fillId="360" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="361" fillId="362" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="363" fillId="364" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="365" fillId="366" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="367" fillId="368" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="369" fillId="370" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="371" fillId="372" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="373" fillId="374" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="375" fillId="376" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="377" fillId="378" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="379" fillId="380" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="381" fillId="382" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="383" fillId="384" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="385" fillId="386" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="387" fillId="388" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="389" fillId="390" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="391" fillId="392" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="393" fillId="394" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="395" fillId="396" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="397" fillId="398" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="399" fillId="400" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="401" fillId="402" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="403" fillId="404" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="405" fillId="406" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="407" fillId="408" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="409" fillId="410" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="411" fillId="412" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="413" fillId="414" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="415" fillId="416" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="417" fillId="418" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="419" fillId="420" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="421" fillId="422" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="423" fillId="424" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="425" fillId="426" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="427" fillId="428" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="429" fillId="430" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="431" fillId="432" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="433" fillId="434" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="435" fillId="436" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="437" fillId="438" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="439" fillId="440" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="441" fillId="442" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="443" fillId="444" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="445" fillId="446" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="447" fillId="448" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="449" fillId="450" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="451" fillId="452" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="453" fillId="454" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="455" fillId="456" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="457" fillId="458" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="459" fillId="460" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="461" fillId="462" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="463" fillId="464" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="465" fillId="466" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="467" fillId="468" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="469" fillId="470" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="471" fillId="472" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="473" fillId="474" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="475" fillId="476" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="477" fillId="478" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="479" fillId="480" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="481" fillId="482" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="483" fillId="484" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="485" fillId="486" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="487" fillId="488" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="489" fillId="490" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="491" fillId="492" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="493" fillId="494" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="495" fillId="496" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="497" fillId="498" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="499" fillId="500" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="501" fillId="502" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="503" fillId="504" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="505" fillId="506" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="507" fillId="508" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="509" fillId="510" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="511" fillId="512" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="513" fillId="514" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="515" fillId="516" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="517" fillId="518" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="519" fillId="520" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="521" fillId="522" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="523" fillId="524" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="525" fillId="526" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="527" fillId="528" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="529" fillId="530" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="531" fillId="532" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="533" fillId="534" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="535" fillId="536" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="537" fillId="538" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="539" fillId="540" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="541" fillId="542" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="543" fillId="544" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="545" fillId="546" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="547" fillId="548" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="549" fillId="550" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="551" fillId="552" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="553" fillId="554" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="555" fillId="556" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="557" fillId="558" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="559" fillId="560" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="561" fillId="562" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="563" fillId="564" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="565" fillId="566" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="567" fillId="568" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="569" fillId="570" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="571" fillId="572" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="573" fillId="574" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="576" borderId="575" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -2874,8 +5946,8 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.73046875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.98046875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="41.12109375" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" style="13" width="6.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="13" width="7.28515625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
@@ -2942,11 +6014,11 @@
       <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="126" t="s">
-        <v>51</v>
+      <c r="C2" s="295" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="294" t="s">
+        <v>67</v>
       </c>
       <c r="E2" s="11">
         <v>1</v>
@@ -2989,11 +6061,11 @@
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="129" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="128" t="s">
-        <v>51</v>
+      <c r="C3" s="297" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="296" t="s">
+        <v>67</v>
       </c>
       <c r="E3" s="12">
         <v>400</v>
@@ -3036,11 +6108,11 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="131" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="130" t="s">
-        <v>51</v>
+      <c r="C4" s="299" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="298" t="s">
+        <v>67</v>
       </c>
       <c r="E4" s="12">
         <v>400</v>
@@ -3083,11 +6155,11 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="133" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="132" t="s">
-        <v>51</v>
+      <c r="C5" s="301" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="300" t="s">
+        <v>67</v>
       </c>
       <c r="E5" s="12">
         <v>400</v>
@@ -3130,11 +6202,11 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="135" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="134" t="s">
-        <v>51</v>
+      <c r="C6" s="303" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="302" t="s">
+        <v>67</v>
       </c>
       <c r="E6" s="12">
         <v>156.47999999999999</v>
@@ -3177,11 +6249,11 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="137" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="136" t="s">
-        <v>51</v>
+      <c r="C7" s="305" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="304" t="s">
+        <v>67</v>
       </c>
       <c r="E7" s="12">
         <v>1</v>
@@ -3224,11 +6296,11 @@
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="139" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="138" t="s">
-        <v>51</v>
+      <c r="C8" s="307" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="306" t="s">
+        <v>67</v>
       </c>
       <c r="E8" s="7">
         <v>2000</v>

</xml_diff>

<commit_message>
segrigation of qa and stg
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
+++ b/binaries/FCfiles/ManageBilling/ManageBilling.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -306,7 +306,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="633">
+  <fills count="857">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3469,8 +3469,1128 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="632">
+  <borders count="856">
     <border>
       <left/>
       <right/>
@@ -5803,11 +6923,795 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="336">
+  <cellXfs count="448">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
@@ -6149,7 +8053,119 @@
     <xf applyBorder="true" applyFill="true" borderId="625" fillId="626" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="627" fillId="628" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="629" fillId="630" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="632" borderId="631" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="631" fillId="632" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="633" fillId="634" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="635" fillId="636" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="637" fillId="638" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="639" fillId="640" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="641" fillId="642" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="643" fillId="644" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="645" fillId="646" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="647" fillId="648" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="649" fillId="650" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="651" fillId="652" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="653" fillId="654" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="655" fillId="656" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="657" fillId="658" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="659" fillId="660" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="661" fillId="662" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="663" fillId="664" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="665" fillId="666" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="667" fillId="668" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="669" fillId="670" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="671" fillId="672" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="673" fillId="674" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="675" fillId="676" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="677" fillId="678" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="679" fillId="680" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="681" fillId="682" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="683" fillId="684" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="685" fillId="686" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="687" fillId="688" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="689" fillId="690" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="691" fillId="692" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="693" fillId="694" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="695" fillId="696" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="697" fillId="698" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="699" fillId="700" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="701" fillId="702" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="703" fillId="704" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="705" fillId="706" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="707" fillId="708" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="709" fillId="710" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="711" fillId="712" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="713" fillId="714" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="715" fillId="716" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="717" fillId="718" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="719" fillId="720" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="721" fillId="722" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="723" fillId="724" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="725" fillId="726" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="727" fillId="728" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="729" fillId="730" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="731" fillId="732" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="733" fillId="734" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="735" fillId="736" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="737" fillId="738" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="739" fillId="740" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="741" fillId="742" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="743" fillId="744" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="745" fillId="746" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="747" fillId="748" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="749" fillId="750" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="751" fillId="752" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="753" fillId="754" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="755" fillId="756" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="757" fillId="758" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="759" fillId="760" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="761" fillId="762" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="763" fillId="764" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="765" fillId="766" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="767" fillId="768" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="769" fillId="770" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="771" fillId="772" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="773" fillId="774" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="775" fillId="776" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="777" fillId="778" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="779" fillId="780" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="781" fillId="782" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="783" fillId="784" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="785" fillId="786" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="787" fillId="788" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="789" fillId="790" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="791" fillId="792" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="793" fillId="794" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="795" fillId="796" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="797" fillId="798" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="799" fillId="800" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="801" fillId="802" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="803" fillId="804" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="805" fillId="806" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="807" fillId="808" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="809" fillId="810" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="811" fillId="812" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="813" fillId="814" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="815" fillId="816" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="817" fillId="818" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="819" fillId="820" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="821" fillId="822" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="823" fillId="824" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="825" fillId="826" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="827" fillId="828" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="829" fillId="830" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="831" fillId="832" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="833" fillId="834" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="835" fillId="836" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="837" fillId="838" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="839" fillId="840" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="841" fillId="842" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="843" fillId="844" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="845" fillId="846" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="847" fillId="848" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="849" fillId="850" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="851" fillId="852" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="853" fillId="854" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="856" borderId="855" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -6566,10 +8582,10 @@
       <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="323" t="s">
+      <c r="C2" s="435" t="s">
         <v>84</v>
       </c>
-      <c r="D2" s="322" t="s">
+      <c r="D2" s="434" t="s">
         <v>83</v>
       </c>
       <c r="E2" s="11">
@@ -6613,10 +8629,10 @@
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="325" t="s">
+      <c r="C3" s="437" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="324" t="s">
+      <c r="D3" s="436" t="s">
         <v>83</v>
       </c>
       <c r="E3" s="12">
@@ -6660,10 +8676,10 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="327" t="s">
+      <c r="C4" s="439" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="326" t="s">
+      <c r="D4" s="438" t="s">
         <v>83</v>
       </c>
       <c r="E4" s="12">
@@ -6707,10 +8723,10 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="329" t="s">
+      <c r="C5" s="441" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="328" t="s">
+      <c r="D5" s="440" t="s">
         <v>83</v>
       </c>
       <c r="E5" s="12">
@@ -6754,10 +8770,10 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="331" t="s">
+      <c r="C6" s="443" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="330" t="s">
+      <c r="D6" s="442" t="s">
         <v>83</v>
       </c>
       <c r="E6" s="12">
@@ -6801,10 +8817,10 @@
       <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="333" t="s">
+      <c r="C7" s="445" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="332" t="s">
+      <c r="D7" s="444" t="s">
         <v>83</v>
       </c>
       <c r="E7" s="12">
@@ -6848,10 +8864,10 @@
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="335" t="s">
+      <c r="C8" s="447" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="334" t="s">
+      <c r="D8" s="446" t="s">
         <v>83</v>
       </c>
       <c r="E8" s="7">

</xml_diff>